<commit_message>
City index update, 4/12.
</commit_message>
<xml_diff>
--- a/data_indexpoints_tidy/tallmateriale_19954.xlsx
+++ b/data_indexpoints_tidy/tallmateriale_19954.xlsx
@@ -1735,19 +1735,19 @@
         <v>2025</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="E2">
-        <v>1.0102</v>
+        <v>1.0128</v>
       </c>
       <c r="F2">
         <v>11</v>
       </c>
       <c r="G2">
-        <v>1.059319789667317</v>
+        <v>1.14674855465626</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -1766,19 +1766,19 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>mai</t>
+          <t>jun</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>jan-mai</t>
+          <t>jan-jun</t>
         </is>
       </c>
       <c r="M2">
-        <v>-1.1</v>
+        <v>-0.9</v>
       </c>
       <c r="N2">
-        <v>3.1</v>
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>
@@ -1788,7 +1788,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H173"/>
+  <dimension ref="A1:H181"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2067,16 +2067,16 @@
         <v>2024</v>
       </c>
       <c r="D10">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E10">
-        <v>100</v>
+        <v>99.98751092793806</v>
       </c>
       <c r="F10">
-        <v>100</v>
+        <v>99.98751092793805</v>
       </c>
       <c r="G10">
-        <v>1013</v>
+        <v>7398</v>
       </c>
     </row>
     <row r="11">
@@ -2094,16 +2094,16 @@
         <v>2024</v>
       </c>
       <c r="D11">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E11">
-        <v>99.98751092793806</v>
+        <v>100</v>
       </c>
       <c r="F11">
-        <v>99.98751092793805</v>
+        <v>100</v>
       </c>
       <c r="G11">
-        <v>7398</v>
+        <v>6515</v>
       </c>
     </row>
     <row r="12">
@@ -2118,19 +2118,22 @@
         </is>
       </c>
       <c r="C12">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D12">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>100</v>
+        <v>99.98621450234354</v>
       </c>
       <c r="F12">
-        <v>100</v>
+        <v>99.98621450234354</v>
       </c>
       <c r="G12">
-        <v>6515</v>
+        <v>6720</v>
+      </c>
+      <c r="H12">
+        <v>2.45</v>
       </c>
     </row>
     <row r="13">
@@ -2148,19 +2151,19 @@
         <v>2025</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13">
-        <v>99.98621450234354</v>
+        <v>99.98692639560726</v>
       </c>
       <c r="F13">
-        <v>99.98621450234354</v>
+        <v>99.98692639560727</v>
       </c>
       <c r="G13">
-        <v>6720</v>
+        <v>7097</v>
       </c>
       <c r="H13">
-        <v>2.45</v>
+        <v>4.03</v>
       </c>
     </row>
     <row r="14">
@@ -2178,19 +2181,19 @@
         <v>2025</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E14">
-        <v>99.98692639560726</v>
+        <v>100</v>
       </c>
       <c r="F14">
-        <v>99.98692639560727</v>
+        <v>100</v>
       </c>
       <c r="G14">
-        <v>7097</v>
+        <v>6823</v>
       </c>
       <c r="H14">
-        <v>4.03</v>
+        <v>6.53</v>
       </c>
     </row>
     <row r="15">
@@ -2208,7 +2211,7 @@
         <v>2025</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E15">
         <v>100</v>
@@ -2217,10 +2220,10 @@
         <v>100</v>
       </c>
       <c r="G15">
-        <v>6823</v>
+        <v>6834</v>
       </c>
       <c r="H15">
-        <v>6.53</v>
+        <v>-8.449999999999999</v>
       </c>
     </row>
     <row r="16">
@@ -2238,19 +2241,19 @@
         <v>2025</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E16">
-        <v>100</v>
+        <v>99.98805684939687</v>
       </c>
       <c r="F16">
-        <v>100</v>
+        <v>99.98805684939687</v>
       </c>
       <c r="G16">
-        <v>6834</v>
+        <v>7664</v>
       </c>
       <c r="H16">
-        <v>-8.449999999999999</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="17">
@@ -2268,19 +2271,19 @@
         <v>2025</v>
       </c>
       <c r="D17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E17">
-        <v>99.98805684939687</v>
+        <v>100</v>
       </c>
       <c r="F17">
-        <v>99.98805684939687</v>
+        <v>100</v>
       </c>
       <c r="G17">
-        <v>7664</v>
+        <v>7871</v>
       </c>
       <c r="H17">
-        <v>1.25</v>
+        <v>2.04</v>
       </c>
     </row>
     <row r="18">
@@ -2514,16 +2517,16 @@
         <v>2024</v>
       </c>
       <c r="D26">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E26">
-        <v>100</v>
+        <v>99.98760996159089</v>
       </c>
       <c r="F26">
-        <v>100</v>
+        <v>99.98760996159089</v>
       </c>
       <c r="G26">
-        <v>956</v>
+        <v>7406</v>
       </c>
     </row>
     <row r="27">
@@ -2541,16 +2544,16 @@
         <v>2024</v>
       </c>
       <c r="D27">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E27">
-        <v>99.98760996159089</v>
+        <v>100</v>
       </c>
       <c r="F27">
-        <v>99.98760996159089</v>
+        <v>100</v>
       </c>
       <c r="G27">
-        <v>7406</v>
+        <v>6547</v>
       </c>
     </row>
     <row r="28">
@@ -2565,19 +2568,22 @@
         </is>
       </c>
       <c r="C28">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D28">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E28">
-        <v>100</v>
+        <v>99.98635743519782</v>
       </c>
       <c r="F28">
-        <v>100</v>
+        <v>99.98635743519782</v>
       </c>
       <c r="G28">
-        <v>6547</v>
+        <v>6760</v>
+      </c>
+      <c r="H28">
+        <v>0.1</v>
       </c>
     </row>
     <row r="29">
@@ -2595,19 +2601,19 @@
         <v>2025</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29">
-        <v>99.98635743519782</v>
+        <v>99.98686457375541</v>
       </c>
       <c r="F29">
-        <v>99.98635743519782</v>
+        <v>99.98686457375541</v>
       </c>
       <c r="G29">
-        <v>6760</v>
+        <v>7025</v>
       </c>
       <c r="H29">
-        <v>0.1</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="30">
@@ -2625,19 +2631,19 @@
         <v>2025</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E30">
-        <v>99.98686457375541</v>
+        <v>99.98664173123163</v>
       </c>
       <c r="F30">
-        <v>99.98686457375541</v>
+        <v>99.98664173123163</v>
       </c>
       <c r="G30">
-        <v>7025</v>
+        <v>6896</v>
       </c>
       <c r="H30">
-        <v>0.24</v>
+        <v>3.56</v>
       </c>
     </row>
     <row r="31">
@@ -2655,19 +2661,19 @@
         <v>2025</v>
       </c>
       <c r="D31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E31">
-        <v>99.98664173123163</v>
+        <v>99.98654829163304</v>
       </c>
       <c r="F31">
-        <v>99.98664173123163</v>
+        <v>99.98654829163304</v>
       </c>
       <c r="G31">
-        <v>6896</v>
+        <v>6863</v>
       </c>
       <c r="H31">
-        <v>3.56</v>
+        <v>-11.15</v>
       </c>
     </row>
     <row r="32">
@@ -2685,19 +2691,19 @@
         <v>2025</v>
       </c>
       <c r="D32">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E32">
-        <v>99.98654829163304</v>
+        <v>99.97624138750297</v>
       </c>
       <c r="F32">
-        <v>99.98654829163304</v>
+        <v>99.97624138750297</v>
       </c>
       <c r="G32">
-        <v>6863</v>
+        <v>7667</v>
       </c>
       <c r="H32">
-        <v>-11.15</v>
+        <v>-0.51</v>
       </c>
     </row>
     <row r="33">
@@ -2715,19 +2721,19 @@
         <v>2025</v>
       </c>
       <c r="D33">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E33">
-        <v>99.97624138750297</v>
+        <v>99.97739091114627</v>
       </c>
       <c r="F33">
-        <v>99.97624138750297</v>
+        <v>99.97739091114627</v>
       </c>
       <c r="G33">
-        <v>7667</v>
+        <v>7961</v>
       </c>
       <c r="H33">
-        <v>-0.51</v>
+        <v>3.18</v>
       </c>
     </row>
     <row r="34">
@@ -3207,28 +3213,31 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>86957V885288</t>
+          <t>43264V886007</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Jernbaneveien</t>
+          <t>Hunstad</t>
         </is>
       </c>
       <c r="C51">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E51">
-        <v>99.94874423372629</v>
+        <v>99.98230401698815</v>
       </c>
       <c r="F51">
-        <v>99.94874423372629</v>
+        <v>99.98230401698814</v>
       </c>
       <c r="G51">
-        <v>6542</v>
+        <v>20491</v>
+      </c>
+      <c r="H51">
+        <v>2.34</v>
       </c>
     </row>
     <row r="52">
@@ -3246,16 +3255,16 @@
         <v>2024</v>
       </c>
       <c r="D52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E52">
-        <v>99.96293550778356</v>
+        <v>99.94874423372629</v>
       </c>
       <c r="F52">
-        <v>99.96293550778354</v>
+        <v>99.94874423372629</v>
       </c>
       <c r="G52">
-        <v>6759</v>
+        <v>6542</v>
       </c>
     </row>
     <row r="53">
@@ -3273,16 +3282,16 @@
         <v>2024</v>
       </c>
       <c r="D53">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E53">
-        <v>50.94643502284561</v>
+        <v>99.96293550778356</v>
       </c>
       <c r="F53">
-        <v>98.71427053448093</v>
+        <v>99.96293550778354</v>
       </c>
       <c r="G53">
-        <v>7856</v>
+        <v>6759</v>
       </c>
     </row>
     <row r="54">
@@ -3300,16 +3309,16 @@
         <v>2024</v>
       </c>
       <c r="D54">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E54">
-        <v>98.59620148637491</v>
+        <v>50.94643502284561</v>
       </c>
       <c r="F54">
-        <v>98.59620148637489</v>
+        <v>98.71427053448093</v>
       </c>
       <c r="G54">
-        <v>7879</v>
+        <v>7856</v>
       </c>
     </row>
     <row r="55">
@@ -3327,16 +3336,16 @@
         <v>2024</v>
       </c>
       <c r="D55">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E55">
-        <v>98.75123233651001</v>
+        <v>98.59620148637491</v>
       </c>
       <c r="F55">
-        <v>98.75123233651001</v>
+        <v>98.59620148637489</v>
       </c>
       <c r="G55">
-        <v>7473</v>
+        <v>7879</v>
       </c>
     </row>
     <row r="56">
@@ -3354,16 +3363,16 @@
         <v>2024</v>
       </c>
       <c r="D56">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E56">
-        <v>99.1095965702979</v>
+        <v>98.75123233651001</v>
       </c>
       <c r="F56">
-        <v>99.1095965702979</v>
+        <v>98.75123233651001</v>
       </c>
       <c r="G56">
-        <v>7499</v>
+        <v>7473</v>
       </c>
     </row>
     <row r="57">
@@ -3381,16 +3390,16 @@
         <v>2024</v>
       </c>
       <c r="D57">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E57">
-        <v>99.72160356347439</v>
+        <v>99.1095965702979</v>
       </c>
       <c r="F57">
-        <v>99.72160356347439</v>
+        <v>99.1095965702979</v>
       </c>
       <c r="G57">
-        <v>7501</v>
+        <v>7499</v>
       </c>
     </row>
     <row r="58">
@@ -3408,16 +3417,16 @@
         <v>2024</v>
       </c>
       <c r="D58">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E58">
-        <v>99.95003747189608</v>
+        <v>99.72160356347439</v>
       </c>
       <c r="F58">
-        <v>99.95003747189608</v>
+        <v>99.72160356347439</v>
       </c>
       <c r="G58">
-        <v>6681</v>
+        <v>7501</v>
       </c>
     </row>
     <row r="59">
@@ -3435,16 +3444,16 @@
         <v>2024</v>
       </c>
       <c r="D59">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E59">
-        <v>99.95759717314488</v>
+        <v>99.95003747189608</v>
       </c>
       <c r="F59">
-        <v>99.95759717314488</v>
+        <v>99.95003747189608</v>
       </c>
       <c r="G59">
-        <v>6057</v>
+        <v>6681</v>
       </c>
     </row>
     <row r="60">
@@ -3459,22 +3468,19 @@
         </is>
       </c>
       <c r="C60">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D60">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E60">
-        <v>99.97612510445268</v>
+        <v>99.95759717314488</v>
       </c>
       <c r="F60">
-        <v>99.97612510445268</v>
+        <v>99.95759717314488</v>
       </c>
       <c r="G60">
-        <v>6911</v>
-      </c>
-      <c r="H60">
-        <v>5.64</v>
+        <v>6057</v>
       </c>
     </row>
     <row r="61">
@@ -3492,19 +3498,19 @@
         <v>2025</v>
       </c>
       <c r="D61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E61">
-        <v>99.94329136894633</v>
+        <v>99.97612510445268</v>
       </c>
       <c r="F61">
-        <v>99.94329136894635</v>
+        <v>99.97612510445268</v>
       </c>
       <c r="G61">
-        <v>7387</v>
+        <v>6911</v>
       </c>
       <c r="H61">
-        <v>9.57</v>
+        <v>5.64</v>
       </c>
     </row>
     <row r="62">
@@ -3522,16 +3528,19 @@
         <v>2025</v>
       </c>
       <c r="D62">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E62">
-        <v>99.93048314216198</v>
+        <v>99.94329136894633</v>
       </c>
       <c r="F62">
-        <v>99.93048314216198</v>
+        <v>99.94329136894635</v>
       </c>
       <c r="G62">
-        <v>7220</v>
+        <v>7387</v>
+      </c>
+      <c r="H62">
+        <v>9.57</v>
       </c>
     </row>
     <row r="63">
@@ -3549,16 +3558,16 @@
         <v>2025</v>
       </c>
       <c r="D63">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E63">
-        <v>96.37458157028679</v>
+        <v>99.93048314216198</v>
       </c>
       <c r="F63">
-        <v>99.69440526563234</v>
+        <v>99.93048314216198</v>
       </c>
       <c r="G63">
-        <v>7158</v>
+        <v>7220</v>
       </c>
     </row>
     <row r="64">
@@ -3576,43 +3585,43 @@
         <v>2025</v>
       </c>
       <c r="D64">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E64">
-        <v>95.99191251076863</v>
+        <v>96.37458157028679</v>
       </c>
       <c r="F64">
-        <v>99.19594141858907</v>
+        <v>99.69440526563234</v>
       </c>
       <c r="G64">
-        <v>8751</v>
+        <v>7158</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>08422V886041</t>
+          <t>86957V885288</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Kirkeveien v/Reinslettkrysset</t>
+          <t>Jernbaneveien</t>
         </is>
       </c>
       <c r="C65">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D65">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E65">
-        <v>98.53252247488101</v>
+        <v>99.97276193934994</v>
       </c>
       <c r="F65">
-        <v>98.53252247488101</v>
+        <v>99.97276193934992</v>
       </c>
       <c r="G65">
-        <v>7140</v>
+        <v>9202</v>
       </c>
     </row>
     <row r="66">
@@ -3630,16 +3639,16 @@
         <v>2024</v>
       </c>
       <c r="D66">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E66">
-        <v>98.90137328339576</v>
+        <v>98.53252247488101</v>
       </c>
       <c r="F66">
-        <v>98.90137328339576</v>
+        <v>98.53252247488101</v>
       </c>
       <c r="G66">
-        <v>7418</v>
+        <v>7140</v>
       </c>
     </row>
     <row r="67">
@@ -3657,16 +3666,16 @@
         <v>2024</v>
       </c>
       <c r="D67">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E67">
-        <v>98.50953701527615</v>
+        <v>98.90137328339576</v>
       </c>
       <c r="F67">
-        <v>98.51938895417156</v>
+        <v>98.90137328339576</v>
       </c>
       <c r="G67">
-        <v>8006</v>
+        <v>7418</v>
       </c>
     </row>
     <row r="68">
@@ -3681,22 +3690,19 @@
         </is>
       </c>
       <c r="C68">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D68">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E68">
-        <v>98.53018372703411</v>
+        <v>98.50953701527615</v>
       </c>
       <c r="F68">
-        <v>98.53018372703411</v>
+        <v>98.51938895417156</v>
       </c>
       <c r="G68">
-        <v>7211</v>
-      </c>
-      <c r="H68">
-        <v>-1.61</v>
+        <v>8006</v>
       </c>
     </row>
     <row r="69">
@@ -3714,19 +3720,19 @@
         <v>2025</v>
       </c>
       <c r="D69">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E69">
-        <v>98.73186037390509</v>
+        <v>98.53018372703411</v>
       </c>
       <c r="F69">
-        <v>98.73186037390509</v>
+        <v>98.53018372703411</v>
       </c>
       <c r="G69">
-        <v>7268</v>
+        <v>7211</v>
       </c>
       <c r="H69">
-        <v>0.68</v>
+        <v>-1.61</v>
       </c>
     </row>
     <row r="70">
@@ -3744,19 +3750,19 @@
         <v>2025</v>
       </c>
       <c r="D70">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E70">
-        <v>98.67409175285069</v>
+        <v>98.73186037390509</v>
       </c>
       <c r="F70">
-        <v>98.6740917528507</v>
+        <v>98.73186037390509</v>
       </c>
       <c r="G70">
-        <v>7138</v>
+        <v>7268</v>
       </c>
       <c r="H70">
-        <v>-12.04</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="71">
@@ -3774,73 +3780,79 @@
         <v>2025</v>
       </c>
       <c r="D71">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E71">
-        <v>98.53519113969274</v>
+        <v>98.67409175285069</v>
       </c>
       <c r="F71">
-        <v>98.53519113969274</v>
+        <v>98.6740917528507</v>
       </c>
       <c r="G71">
-        <v>7875</v>
+        <v>7138</v>
       </c>
       <c r="H71">
-        <v>-6.19</v>
+        <v>-12.04</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>18346V886007</t>
+          <t>08422V886041</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Mørkved</t>
+          <t>Kirkeveien v/Reinslettkrysset</t>
         </is>
       </c>
       <c r="C72">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D72">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E72">
-        <v>99.9826914755517</v>
+        <v>98.53519113969274</v>
       </c>
       <c r="F72">
-        <v>99.9826914755517</v>
+        <v>98.53519113969274</v>
       </c>
       <c r="G72">
-        <v>10666</v>
+        <v>7875</v>
+      </c>
+      <c r="H72">
+        <v>-6.19</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>18346V886007</t>
+          <t>08422V886041</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Mørkved</t>
+          <t>Kirkeveien v/Reinslettkrysset</t>
         </is>
       </c>
       <c r="C73">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D73">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E73">
-        <v>99.98411311462388</v>
+        <v>98.58770472347496</v>
       </c>
       <c r="F73">
-        <v>99.98411311462388</v>
+        <v>98.58770472347496</v>
       </c>
       <c r="G73">
-        <v>11640</v>
+        <v>7842</v>
+      </c>
+      <c r="H73">
+        <v>-4.53</v>
       </c>
     </row>
     <row r="74">
@@ -3858,16 +3870,16 @@
         <v>2024</v>
       </c>
       <c r="D74">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E74">
-        <v>99.96826152503372</v>
+        <v>99.9826914755517</v>
       </c>
       <c r="F74">
-        <v>99.96826152503372</v>
+        <v>99.9826914755517</v>
       </c>
       <c r="G74">
-        <v>11679</v>
+        <v>10666</v>
       </c>
     </row>
     <row r="75">
@@ -3885,16 +3897,16 @@
         <v>2024</v>
       </c>
       <c r="D75">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E75">
-        <v>99.95239390642001</v>
+        <v>99.98411311462388</v>
       </c>
       <c r="F75">
-        <v>99.95239390642003</v>
+        <v>99.98411311462388</v>
       </c>
       <c r="G75">
-        <v>13507</v>
+        <v>11640</v>
       </c>
     </row>
     <row r="76">
@@ -3912,16 +3924,16 @@
         <v>2024</v>
       </c>
       <c r="D76">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E76">
-        <v>99.93508601103538</v>
+        <v>99.96826152503372</v>
       </c>
       <c r="F76">
-        <v>99.93508601103538</v>
+        <v>99.96826152503372</v>
       </c>
       <c r="G76">
-        <v>13977</v>
+        <v>11679</v>
       </c>
     </row>
     <row r="77">
@@ -3939,16 +3951,16 @@
         <v>2024</v>
       </c>
       <c r="D77">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E77">
-        <v>99.97513983840894</v>
+        <v>99.95239390642001</v>
       </c>
       <c r="F77">
-        <v>99.97513983840895</v>
+        <v>99.95239390642003</v>
       </c>
       <c r="G77">
-        <v>14443</v>
+        <v>13507</v>
       </c>
     </row>
     <row r="78">
@@ -3966,16 +3978,16 @@
         <v>2024</v>
       </c>
       <c r="D78">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E78">
-        <v>99.98045347928068</v>
+        <v>99.93508601103538</v>
       </c>
       <c r="F78">
-        <v>99.98045347928068</v>
+        <v>99.93508601103538</v>
       </c>
       <c r="G78">
-        <v>13730</v>
+        <v>13977</v>
       </c>
     </row>
     <row r="79">
@@ -3993,16 +4005,16 @@
         <v>2024</v>
       </c>
       <c r="D79">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E79">
-        <v>99.9608916699257</v>
+        <v>99.97513983840894</v>
       </c>
       <c r="F79">
-        <v>99.96089166992569</v>
+        <v>99.97513983840895</v>
       </c>
       <c r="G79">
-        <v>13823</v>
+        <v>14443</v>
       </c>
     </row>
     <row r="80">
@@ -4020,16 +4032,16 @@
         <v>2024</v>
       </c>
       <c r="D80">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E80">
-        <v>99.95318978199813</v>
+        <v>99.98045347928068</v>
       </c>
       <c r="F80">
-        <v>99.95318978199813</v>
+        <v>99.98045347928068</v>
       </c>
       <c r="G80">
-        <v>13504</v>
+        <v>13730</v>
       </c>
     </row>
     <row r="81">
@@ -4047,16 +4059,16 @@
         <v>2024</v>
       </c>
       <c r="D81">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E81">
-        <v>99.95108657675914</v>
+        <v>99.9608916699257</v>
       </c>
       <c r="F81">
-        <v>99.95108657675914</v>
+        <v>99.96089166992569</v>
       </c>
       <c r="G81">
-        <v>13029</v>
+        <v>13823</v>
       </c>
     </row>
     <row r="82">
@@ -4074,16 +4086,16 @@
         <v>2024</v>
       </c>
       <c r="D82">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E82">
-        <v>100</v>
+        <v>99.95318978199813</v>
       </c>
       <c r="F82">
-        <v>100</v>
+        <v>99.95318978199813</v>
       </c>
       <c r="G82">
-        <v>12585</v>
+        <v>13504</v>
       </c>
     </row>
     <row r="83">
@@ -4101,16 +4113,16 @@
         <v>2024</v>
       </c>
       <c r="D83">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E83">
-        <v>100</v>
+        <v>99.95108657675914</v>
       </c>
       <c r="F83">
-        <v>100</v>
+        <v>99.95108657675914</v>
       </c>
       <c r="G83">
-        <v>11520</v>
+        <v>13029</v>
       </c>
     </row>
     <row r="84">
@@ -4125,22 +4137,19 @@
         </is>
       </c>
       <c r="C84">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D84">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E84">
-        <v>99.98398847169963</v>
+        <v>100</v>
       </c>
       <c r="F84">
-        <v>99.98398847169963</v>
+        <v>100</v>
       </c>
       <c r="G84">
-        <v>11574</v>
-      </c>
-      <c r="H84">
-        <v>8.52</v>
+        <v>12585</v>
       </c>
     </row>
     <row r="85">
@@ -4155,22 +4164,19 @@
         </is>
       </c>
       <c r="C85">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D85">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E85">
-        <v>99.98487369535624</v>
+        <v>100</v>
       </c>
       <c r="F85">
-        <v>99.98487369535623</v>
+        <v>100</v>
       </c>
       <c r="G85">
-        <v>12250</v>
-      </c>
-      <c r="H85">
-        <v>5.62</v>
+        <v>11520</v>
       </c>
     </row>
     <row r="86">
@@ -4188,19 +4194,19 @@
         <v>2025</v>
       </c>
       <c r="D86">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E86">
-        <v>99.96985227615315</v>
+        <v>99.98398847169963</v>
       </c>
       <c r="F86">
-        <v>99.96985227615315</v>
+        <v>99.98398847169963</v>
       </c>
       <c r="G86">
-        <v>12283</v>
+        <v>11574</v>
       </c>
       <c r="H86">
-        <v>5.28</v>
+        <v>8.52</v>
       </c>
     </row>
     <row r="87">
@@ -4218,19 +4224,19 @@
         <v>2025</v>
       </c>
       <c r="D87">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E87">
-        <v>99.97812932857039</v>
+        <v>99.98487369535624</v>
       </c>
       <c r="F87">
-        <v>99.97812932857039</v>
+        <v>99.98487369535623</v>
       </c>
       <c r="G87">
-        <v>12693</v>
+        <v>12250</v>
       </c>
       <c r="H87">
-        <v>-6.05</v>
+        <v>5.62</v>
       </c>
     </row>
     <row r="88">
@@ -4248,100 +4254,109 @@
         <v>2025</v>
       </c>
       <c r="D88">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E88">
-        <v>99.96443528283797</v>
+        <v>99.96985227615315</v>
       </c>
       <c r="F88">
-        <v>99.97443272611058</v>
+        <v>99.96985227615315</v>
       </c>
       <c r="G88">
-        <v>14199</v>
+        <v>12283</v>
       </c>
       <c r="H88">
-        <v>1.63</v>
+        <v>5.28</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>24556V1201963</t>
+          <t>18346V886007</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Olav V gate (Bodø lufthavn)</t>
+          <t>Mørkved</t>
         </is>
       </c>
       <c r="C89">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D89">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E89">
-        <v>100</v>
+        <v>99.97812932857039</v>
       </c>
       <c r="F89">
-        <v>100</v>
+        <v>99.97812932857039</v>
       </c>
       <c r="G89">
-        <v>5653</v>
+        <v>12693</v>
+      </c>
+      <c r="H89">
+        <v>-6.05</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>24556V1201963</t>
+          <t>18346V886007</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Olav V gate (Bodø lufthavn)</t>
+          <t>Mørkved</t>
         </is>
       </c>
       <c r="C90">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D90">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E90">
-        <v>99.98549673676578</v>
+        <v>99.96443528283797</v>
       </c>
       <c r="F90">
-        <v>99.98549673676578</v>
+        <v>99.97443272611058</v>
       </c>
       <c r="G90">
-        <v>5942</v>
+        <v>14199</v>
+      </c>
+      <c r="H90">
+        <v>1.63</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>24556V1201963</t>
+          <t>18346V886007</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Olav V gate (Bodø lufthavn)</t>
+          <t>Mørkved</t>
         </is>
       </c>
       <c r="C91">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D91">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E91">
-        <v>99.96825396825398</v>
+        <v>99.95789726933717</v>
       </c>
       <c r="F91">
-        <v>99.96825396825398</v>
+        <v>99.95789726933718</v>
       </c>
       <c r="G91">
-        <v>5464</v>
+        <v>14930</v>
+      </c>
+      <c r="H91">
+        <v>3.38</v>
       </c>
     </row>
     <row r="92">
@@ -4359,16 +4374,16 @@
         <v>2024</v>
       </c>
       <c r="D92">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E92">
-        <v>99.97201623058626</v>
+        <v>100</v>
       </c>
       <c r="F92">
-        <v>99.97201623058626</v>
+        <v>100</v>
       </c>
       <c r="G92">
-        <v>6162</v>
+        <v>5653</v>
       </c>
     </row>
     <row r="93">
@@ -4386,16 +4401,16 @@
         <v>2024</v>
       </c>
       <c r="D93">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E93">
-        <v>99.98559285405561</v>
+        <v>99.98549673676578</v>
       </c>
       <c r="F93">
-        <v>99.98559285405561</v>
+        <v>99.98549673676578</v>
       </c>
       <c r="G93">
-        <v>5963</v>
+        <v>5942</v>
       </c>
     </row>
     <row r="94">
@@ -4413,16 +4428,16 @@
         <v>2024</v>
       </c>
       <c r="D94">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E94">
-        <v>99.98634066384375</v>
+        <v>99.96825396825398</v>
       </c>
       <c r="F94">
-        <v>99.98634066384375</v>
+        <v>99.96825396825398</v>
       </c>
       <c r="G94">
-        <v>6256</v>
+        <v>5464</v>
       </c>
     </row>
     <row r="95">
@@ -4440,16 +4455,16 @@
         <v>2024</v>
       </c>
       <c r="D95">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E95">
-        <v>100</v>
+        <v>99.97201623058626</v>
       </c>
       <c r="F95">
-        <v>100</v>
+        <v>99.97201623058626</v>
       </c>
       <c r="G95">
-        <v>5399</v>
+        <v>6162</v>
       </c>
     </row>
     <row r="96">
@@ -4467,16 +4482,16 @@
         <v>2024</v>
       </c>
       <c r="D96">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E96">
-        <v>99.98552612534375</v>
+        <v>99.98559285405561</v>
       </c>
       <c r="F96">
-        <v>99.98552612534375</v>
+        <v>99.98559285405561</v>
       </c>
       <c r="G96">
-        <v>5914</v>
+        <v>5963</v>
       </c>
     </row>
     <row r="97">
@@ -4494,16 +4509,16 @@
         <v>2024</v>
       </c>
       <c r="D97">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E97">
-        <v>100</v>
+        <v>99.98634066384375</v>
       </c>
       <c r="F97">
-        <v>100</v>
+        <v>99.98634066384375</v>
       </c>
       <c r="G97">
-        <v>6550</v>
+        <v>6256</v>
       </c>
     </row>
     <row r="98">
@@ -4521,16 +4536,16 @@
         <v>2024</v>
       </c>
       <c r="D98">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E98">
-        <v>99.98721881390593</v>
+        <v>100</v>
       </c>
       <c r="F98">
-        <v>99.98721881390593</v>
+        <v>100</v>
       </c>
       <c r="G98">
-        <v>6706</v>
+        <v>5399</v>
       </c>
     </row>
     <row r="99">
@@ -4548,16 +4563,16 @@
         <v>2024</v>
       </c>
       <c r="D99">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E99">
-        <v>100</v>
+        <v>99.98552612534375</v>
       </c>
       <c r="F99">
-        <v>100</v>
+        <v>99.98552612534375</v>
       </c>
       <c r="G99">
-        <v>6490</v>
+        <v>5914</v>
       </c>
     </row>
     <row r="100">
@@ -4575,16 +4590,16 @@
         <v>2024</v>
       </c>
       <c r="D100">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E100">
-        <v>99.98447687053709</v>
+        <v>100</v>
       </c>
       <c r="F100">
-        <v>99.98447687053709</v>
+        <v>100</v>
       </c>
       <c r="G100">
-        <v>5620</v>
+        <v>6550</v>
       </c>
     </row>
     <row r="101">
@@ -4599,22 +4614,19 @@
         </is>
       </c>
       <c r="C101">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D101">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E101">
-        <v>99.9854227405248</v>
+        <v>99.98721881390593</v>
       </c>
       <c r="F101">
-        <v>99.98542274052478</v>
+        <v>99.98721881390593</v>
       </c>
       <c r="G101">
-        <v>5839</v>
-      </c>
-      <c r="H101">
-        <v>3.29</v>
+        <v>6706</v>
       </c>
     </row>
     <row r="102">
@@ -4629,22 +4641,19 @@
         </is>
       </c>
       <c r="C102">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D102">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E102">
-        <v>99.98999999999999</v>
+        <v>100</v>
       </c>
       <c r="F102">
         <v>100</v>
       </c>
       <c r="G102">
-        <v>6111</v>
-      </c>
-      <c r="H102">
-        <v>3.31</v>
+        <v>6490</v>
       </c>
     </row>
     <row r="103">
@@ -4659,22 +4668,19 @@
         </is>
       </c>
       <c r="C103">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D103">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E103">
-        <v>100</v>
+        <v>99.98447687053709</v>
       </c>
       <c r="F103">
-        <v>100</v>
+        <v>99.98447687053709</v>
       </c>
       <c r="G103">
-        <v>6164</v>
-      </c>
-      <c r="H103">
-        <v>12.79</v>
+        <v>5620</v>
       </c>
     </row>
     <row r="104">
@@ -4692,19 +4698,19 @@
         <v>2025</v>
       </c>
       <c r="D104">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E104">
-        <v>100</v>
+        <v>99.9854227405248</v>
       </c>
       <c r="F104">
-        <v>100</v>
+        <v>99.98542274052478</v>
       </c>
       <c r="G104">
-        <v>5821</v>
+        <v>5839</v>
       </c>
       <c r="H104">
-        <v>-5.58</v>
+        <v>3.29</v>
       </c>
     </row>
     <row r="105">
@@ -4722,127 +4728,139 @@
         <v>2025</v>
       </c>
       <c r="D105">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E105">
-        <v>99.98593728027001</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="F105">
-        <v>99.98593728027001</v>
+        <v>100</v>
       </c>
       <c r="G105">
-        <v>6085</v>
+        <v>6111</v>
       </c>
       <c r="H105">
-        <v>2.04</v>
+        <v>3.31</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>90646V1201961</t>
+          <t>24556V1201963</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Olav V gate v/byggmakker</t>
+          <t>Olav V gate (Bodø lufthavn)</t>
         </is>
       </c>
       <c r="C106">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D106">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E106">
-        <v>99.93714644877437</v>
+        <v>100</v>
       </c>
       <c r="F106">
-        <v>99.93714644877436</v>
+        <v>100</v>
       </c>
       <c r="G106">
-        <v>8804</v>
+        <v>6164</v>
+      </c>
+      <c r="H106">
+        <v>12.79</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>90646V1201961</t>
+          <t>24556V1201963</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Olav V gate v/byggmakker</t>
+          <t>Olav V gate (Bodø lufthavn)</t>
         </is>
       </c>
       <c r="C107">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D107">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E107">
-        <v>99.90984673945708</v>
+        <v>100</v>
       </c>
       <c r="F107">
-        <v>99.90984673945708</v>
+        <v>100</v>
       </c>
       <c r="G107">
-        <v>9243</v>
+        <v>5821</v>
+      </c>
+      <c r="H107">
+        <v>-5.58</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>90646V1201961</t>
+          <t>24556V1201963</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Olav V gate v/byggmakker</t>
+          <t>Olav V gate (Bodø lufthavn)</t>
         </is>
       </c>
       <c r="C108">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D108">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E108">
-        <v>99.9567894566274</v>
+        <v>99.98593728027001</v>
       </c>
       <c r="F108">
-        <v>99.95678945662742</v>
+        <v>99.98593728027001</v>
       </c>
       <c r="G108">
-        <v>8599</v>
+        <v>6085</v>
+      </c>
+      <c r="H108">
+        <v>2.04</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>90646V1201961</t>
+          <t>24556V1201963</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Olav V gate v/byggmakker</t>
+          <t>Olav V gate (Bodø lufthavn)</t>
         </is>
       </c>
       <c r="C109">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D109">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E109">
-        <v>99.90664675130694</v>
+        <v>99.98633693127476</v>
       </c>
       <c r="F109">
-        <v>99.90664675130695</v>
+        <v>99.98633693127476</v>
       </c>
       <c r="G109">
-        <v>9907</v>
+        <v>6314</v>
+      </c>
+      <c r="H109">
+        <v>0.92</v>
       </c>
     </row>
     <row r="110">
@@ -4860,16 +4878,16 @@
         <v>2024</v>
       </c>
       <c r="D110">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E110">
-        <v>99.87593052109182</v>
+        <v>99.93714644877437</v>
       </c>
       <c r="F110">
-        <v>99.87593052109182</v>
+        <v>99.93714644877436</v>
       </c>
       <c r="G110">
-        <v>9643</v>
+        <v>8804</v>
       </c>
     </row>
     <row r="111">
@@ -4887,16 +4905,16 @@
         <v>2024</v>
       </c>
       <c r="D111">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E111">
-        <v>99.97169544296631</v>
+        <v>99.90984673945708</v>
       </c>
       <c r="F111">
-        <v>99.97169544296631</v>
+        <v>99.90984673945708</v>
       </c>
       <c r="G111">
-        <v>9672</v>
+        <v>9243</v>
       </c>
     </row>
     <row r="112">
@@ -4914,16 +4932,16 @@
         <v>2024</v>
       </c>
       <c r="D112">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E112">
-        <v>99.94468414647638</v>
+        <v>99.9567894566274</v>
       </c>
       <c r="F112">
-        <v>99.94468414647638</v>
+        <v>99.95678945662742</v>
       </c>
       <c r="G112">
-        <v>8224</v>
+        <v>8599</v>
       </c>
     </row>
     <row r="113">
@@ -4941,16 +4959,16 @@
         <v>2024</v>
       </c>
       <c r="D113">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E113">
-        <v>99.9315470369646</v>
+        <v>99.90664675130694</v>
       </c>
       <c r="F113">
-        <v>99.9315470369646</v>
+        <v>99.90664675130695</v>
       </c>
       <c r="G113">
-        <v>9360</v>
+        <v>9907</v>
       </c>
     </row>
     <row r="114">
@@ -4968,16 +4986,16 @@
         <v>2024</v>
       </c>
       <c r="D114">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E114">
-        <v>99.94497432134996</v>
+        <v>99.87593052109182</v>
       </c>
       <c r="F114">
-        <v>99.94497432134996</v>
+        <v>99.87593052109182</v>
       </c>
       <c r="G114">
-        <v>9995</v>
+        <v>9643</v>
       </c>
     </row>
     <row r="115">
@@ -4995,16 +5013,16 @@
         <v>2024</v>
       </c>
       <c r="D115">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E115">
-        <v>99.93634048744998</v>
+        <v>99.97169544296631</v>
       </c>
       <c r="F115">
-        <v>99.93634048744998</v>
+        <v>99.97169544296631</v>
       </c>
       <c r="G115">
-        <v>10074</v>
+        <v>9672</v>
       </c>
     </row>
     <row r="116">
@@ -5022,16 +5040,16 @@
         <v>2024</v>
       </c>
       <c r="D116">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E116">
-        <v>99.95345806571723</v>
+        <v>99.94468414647638</v>
       </c>
       <c r="F116">
-        <v>99.95345806571721</v>
+        <v>99.94468414647638</v>
       </c>
       <c r="G116">
-        <v>9876</v>
+        <v>8224</v>
       </c>
     </row>
     <row r="117">
@@ -5049,16 +5067,16 @@
         <v>2024</v>
       </c>
       <c r="D117">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E117">
-        <v>99.92612137203167</v>
+        <v>99.9315470369646</v>
       </c>
       <c r="F117">
-        <v>99.92612137203166</v>
+        <v>99.9315470369646</v>
       </c>
       <c r="G117">
-        <v>8825</v>
+        <v>9360</v>
       </c>
     </row>
     <row r="118">
@@ -5073,22 +5091,19 @@
         </is>
       </c>
       <c r="C118">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D118">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E118">
-        <v>99.91052788547569</v>
+        <v>99.94497432134996</v>
       </c>
       <c r="F118">
-        <v>99.9105278854757</v>
+        <v>99.94497432134996</v>
       </c>
       <c r="G118">
-        <v>9249</v>
-      </c>
-      <c r="H118">
-        <v>5.05</v>
+        <v>9995</v>
       </c>
     </row>
     <row r="119">
@@ -5103,22 +5118,19 @@
         </is>
       </c>
       <c r="C119">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D119">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E119">
-        <v>99.96229616363466</v>
+        <v>99.93634048744998</v>
       </c>
       <c r="F119">
-        <v>99.96229616363465</v>
+        <v>99.93634048744998</v>
       </c>
       <c r="G119">
-        <v>9773</v>
-      </c>
-      <c r="H119">
-        <v>6.11</v>
+        <v>10074</v>
       </c>
     </row>
     <row r="120">
@@ -5133,22 +5145,19 @@
         </is>
       </c>
       <c r="C120">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D120">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E120">
-        <v>99.96200968752969</v>
+        <v>99.95345806571723</v>
       </c>
       <c r="F120">
-        <v>99.96200968752969</v>
+        <v>99.95345806571721</v>
       </c>
       <c r="G120">
-        <v>9727</v>
-      </c>
-      <c r="H120">
-        <v>13.04</v>
+        <v>9876</v>
       </c>
     </row>
     <row r="121">
@@ -5163,22 +5172,19 @@
         </is>
       </c>
       <c r="C121">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D121">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E121">
-        <v>99.9130182661641</v>
+        <v>99.92612137203167</v>
       </c>
       <c r="F121">
-        <v>99.91301826616412</v>
+        <v>99.92612137203166</v>
       </c>
       <c r="G121">
-        <v>9580</v>
-      </c>
-      <c r="H121">
-        <v>-3.34</v>
+        <v>8825</v>
       </c>
     </row>
     <row r="122">
@@ -5196,154 +5202,169 @@
         <v>2025</v>
       </c>
       <c r="D122">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E122">
-        <v>96.64120230700975</v>
+        <v>99.91052788547569</v>
       </c>
       <c r="F122">
-        <v>99.86690328305235</v>
+        <v>99.9105278854757</v>
       </c>
       <c r="G122">
-        <v>10370</v>
+        <v>9249</v>
       </c>
       <c r="H122">
-        <v>8.210000000000001</v>
+        <v>5.05</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>26549V2669516</t>
+          <t>90646V1201961</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>R80 Olav5 før CityNord</t>
+          <t>Olav V gate v/byggmakker</t>
         </is>
       </c>
       <c r="C123">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D123">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E123">
-        <v>99.91101984941821</v>
+        <v>99.96229616363466</v>
       </c>
       <c r="F123">
-        <v>99.91101984941821</v>
+        <v>99.96229616363465</v>
       </c>
       <c r="G123">
-        <v>13523</v>
+        <v>9773</v>
+      </c>
+      <c r="H123">
+        <v>6.11</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>26549V2669516</t>
+          <t>90646V1201961</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>R80 Olav5 før CityNord</t>
+          <t>Olav V gate v/byggmakker</t>
         </is>
       </c>
       <c r="C124">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D124">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E124">
-        <v>99.94068410993212</v>
+        <v>99.96200968752969</v>
       </c>
       <c r="F124">
-        <v>99.94068410993212</v>
+        <v>99.96200968752969</v>
       </c>
       <c r="G124">
-        <v>14027</v>
+        <v>9727</v>
+      </c>
+      <c r="H124">
+        <v>13.04</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>26549V2669516</t>
+          <t>90646V1201961</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>R80 Olav5 før CityNord</t>
+          <t>Olav V gate v/byggmakker</t>
         </is>
       </c>
       <c r="C125">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D125">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E125">
-        <v>99.91338241663057</v>
+        <v>99.9130182661641</v>
       </c>
       <c r="F125">
-        <v>99.91338241663058</v>
+        <v>99.91301826616412</v>
       </c>
       <c r="G125">
-        <v>12843</v>
+        <v>9580</v>
+      </c>
+      <c r="H125">
+        <v>-3.34</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>26549V2669516</t>
+          <t>90646V1201961</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>R80 Olav5 før CityNord</t>
+          <t>Olav V gate v/byggmakker</t>
         </is>
       </c>
       <c r="C126">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D126">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E126">
-        <v>99.91846973973034</v>
+        <v>96.64120230700975</v>
       </c>
       <c r="F126">
-        <v>99.91846973973033</v>
+        <v>99.86690328305235</v>
       </c>
       <c r="G126">
-        <v>14747</v>
+        <v>10370</v>
+      </c>
+      <c r="H126">
+        <v>8.210000000000001</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>26549V2669516</t>
+          <t>90646V1201961</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>R80 Olav5 før CityNord</t>
+          <t>Olav V gate v/byggmakker</t>
         </is>
       </c>
       <c r="C127">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D127">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E127">
-        <v>99.85389831602039</v>
+        <v>99.93928354584092</v>
       </c>
       <c r="F127">
-        <v>99.88386347506291</v>
+        <v>99.93928354584092</v>
       </c>
       <c r="G127">
-        <v>14250</v>
+        <v>10612</v>
+      </c>
+      <c r="H127">
+        <v>9.66</v>
       </c>
     </row>
     <row r="128">
@@ -5361,16 +5382,16 @@
         <v>2024</v>
       </c>
       <c r="D128">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E128">
-        <v>99.94175888177053</v>
+        <v>99.91101984941821</v>
       </c>
       <c r="F128">
-        <v>99.94175888177053</v>
+        <v>99.91101984941821</v>
       </c>
       <c r="G128">
-        <v>14141</v>
+        <v>13523</v>
       </c>
     </row>
     <row r="129">
@@ -5388,16 +5409,16 @@
         <v>2024</v>
       </c>
       <c r="D129">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E129">
-        <v>99.93991738640631</v>
+        <v>99.94068410993212</v>
       </c>
       <c r="F129">
-        <v>99.93991738640631</v>
+        <v>99.94068410993212</v>
       </c>
       <c r="G129">
-        <v>12159</v>
+        <v>14027</v>
       </c>
     </row>
     <row r="130">
@@ -5415,16 +5436,16 @@
         <v>2024</v>
       </c>
       <c r="D130">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E130">
-        <v>99.94118800235248</v>
+        <v>99.91338241663057</v>
       </c>
       <c r="F130">
-        <v>99.94118800235248</v>
+        <v>99.91338241663058</v>
       </c>
       <c r="G130">
-        <v>14034</v>
+        <v>12843</v>
       </c>
     </row>
     <row r="131">
@@ -5442,16 +5463,16 @@
         <v>2024</v>
       </c>
       <c r="D131">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E131">
-        <v>99.93123710695755</v>
+        <v>99.91846973973034</v>
       </c>
       <c r="F131">
-        <v>99.93123710695755</v>
+        <v>99.91846973973033</v>
       </c>
       <c r="G131">
-        <v>14655</v>
+        <v>14747</v>
       </c>
     </row>
     <row r="132">
@@ -5469,16 +5490,16 @@
         <v>2024</v>
       </c>
       <c r="D132">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E132">
-        <v>99.92129321305322</v>
+        <v>99.85389831602039</v>
       </c>
       <c r="F132">
-        <v>99.92129321305322</v>
+        <v>99.88386347506291</v>
       </c>
       <c r="G132">
-        <v>15181</v>
+        <v>14250</v>
       </c>
     </row>
     <row r="133">
@@ -5496,16 +5517,16 @@
         <v>2024</v>
       </c>
       <c r="D133">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E133">
-        <v>99.91446202724995</v>
+        <v>99.94175888177053</v>
       </c>
       <c r="F133">
-        <v>99.91446202724995</v>
+        <v>99.94175888177053</v>
       </c>
       <c r="G133">
-        <v>15125</v>
+        <v>14141</v>
       </c>
     </row>
     <row r="134">
@@ -5523,16 +5544,16 @@
         <v>2024</v>
       </c>
       <c r="D134">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E134">
-        <v>99.82571390266793</v>
+        <v>99.93991738640631</v>
       </c>
       <c r="F134">
-        <v>99.82571390266793</v>
+        <v>99.93991738640631</v>
       </c>
       <c r="G134">
-        <v>13963</v>
+        <v>12159</v>
       </c>
     </row>
     <row r="135">
@@ -5547,22 +5568,19 @@
         </is>
       </c>
       <c r="C135">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D135">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E135">
-        <v>99.90754193633602</v>
+        <v>99.94118800235248</v>
       </c>
       <c r="F135">
-        <v>99.90754193633602</v>
+        <v>99.94118800235248</v>
       </c>
       <c r="G135">
-        <v>14051</v>
-      </c>
-      <c r="H135">
-        <v>3.9</v>
+        <v>14034</v>
       </c>
     </row>
     <row r="136">
@@ -5577,22 +5595,19 @@
         </is>
       </c>
       <c r="C136">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D136">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E136">
-        <v>99.94245892206382</v>
+        <v>99.93123710695755</v>
       </c>
       <c r="F136">
-        <v>99.94245892206381</v>
+        <v>99.93123710695755</v>
       </c>
       <c r="G136">
-        <v>14489</v>
-      </c>
-      <c r="H136">
-        <v>3.47</v>
+        <v>14655</v>
       </c>
     </row>
     <row r="137">
@@ -5607,22 +5622,19 @@
         </is>
       </c>
       <c r="C137">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D137">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E137">
-        <v>99.94088669950739</v>
+        <v>99.92129321305322</v>
       </c>
       <c r="F137">
-        <v>99.94088669950739</v>
+        <v>99.92129321305322</v>
       </c>
       <c r="G137">
-        <v>14105</v>
-      </c>
-      <c r="H137">
-        <v>9.83</v>
+        <v>15181</v>
       </c>
     </row>
     <row r="138">
@@ -5637,22 +5649,19 @@
         </is>
       </c>
       <c r="C138">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D138">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E138">
-        <v>99.9395323837678</v>
+        <v>99.91446202724995</v>
       </c>
       <c r="F138">
-        <v>99.9395323837678</v>
+        <v>99.91446202724995</v>
       </c>
       <c r="G138">
-        <v>13802</v>
-      </c>
-      <c r="H138">
-        <v>-6.41</v>
+        <v>15125</v>
       </c>
     </row>
     <row r="139">
@@ -5667,184 +5676,199 @@
         </is>
       </c>
       <c r="C139">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D139">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E139">
-        <v>99.92149284377075</v>
+        <v>99.82571390266793</v>
       </c>
       <c r="F139">
-        <v>99.92149284377075</v>
+        <v>99.82571390266793</v>
       </c>
       <c r="G139">
-        <v>15234</v>
-      </c>
-      <c r="H139">
-        <v>7.11</v>
+        <v>13963</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>77027V1207593</t>
+          <t>26549V2669516</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Sjøgata</t>
+          <t>R80 Olav5 før CityNord</t>
         </is>
       </c>
       <c r="C140">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D140">
         <v>1</v>
       </c>
       <c r="E140">
-        <v>99.65114718905139</v>
+        <v>99.90754193633602</v>
       </c>
       <c r="F140">
-        <v>99.65114718905139</v>
+        <v>99.90754193633602</v>
       </c>
       <c r="G140">
-        <v>6722</v>
+        <v>14051</v>
+      </c>
+      <c r="H140">
+        <v>3.9</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>77027V1207593</t>
+          <t>26549V2669516</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Sjøgata</t>
+          <t>R80 Olav5 før CityNord</t>
         </is>
       </c>
       <c r="C141">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D141">
         <v>2</v>
       </c>
       <c r="E141">
-        <v>99.79185638090283</v>
+        <v>99.94245892206382</v>
       </c>
       <c r="F141">
-        <v>99.79185638090283</v>
+        <v>99.94245892206381</v>
       </c>
       <c r="G141">
-        <v>6959</v>
+        <v>14489</v>
+      </c>
+      <c r="H141">
+        <v>3.47</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>77027V1207593</t>
+          <t>26549V2669516</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Sjøgata</t>
+          <t>R80 Olav5 før CityNord</t>
         </is>
       </c>
       <c r="C142">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D142">
         <v>3</v>
       </c>
       <c r="E142">
-        <v>77.28192070242831</v>
+        <v>99.94088669950739</v>
       </c>
       <c r="F142">
-        <v>99.82164906022774</v>
+        <v>99.94088669950739</v>
       </c>
       <c r="G142">
-        <v>6696</v>
+        <v>14105</v>
+      </c>
+      <c r="H142">
+        <v>9.83</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>77027V1207593</t>
+          <t>26549V2669516</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Sjøgata</t>
+          <t>R80 Olav5 før CityNord</t>
         </is>
       </c>
       <c r="C143">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D143">
         <v>4</v>
       </c>
       <c r="E143">
-        <v>99.76520309931909</v>
+        <v>99.9395323837678</v>
       </c>
       <c r="F143">
-        <v>99.76520309931909</v>
+        <v>99.9395323837678</v>
       </c>
       <c r="G143">
-        <v>7773</v>
+        <v>13802</v>
+      </c>
+      <c r="H143">
+        <v>-6.41</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>77027V1207593</t>
+          <t>26549V2669516</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Sjøgata</t>
+          <t>R80 Olav5 før CityNord</t>
         </is>
       </c>
       <c r="C144">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D144">
         <v>5</v>
       </c>
       <c r="E144">
-        <v>99.72764412165229</v>
+        <v>99.92149284377075</v>
       </c>
       <c r="F144">
-        <v>99.72764412165229</v>
+        <v>99.92149284377075</v>
       </c>
       <c r="G144">
-        <v>8008</v>
+        <v>15234</v>
+      </c>
+      <c r="H144">
+        <v>7.11</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>77027V1207593</t>
+          <t>26549V2669516</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Sjøgata</t>
+          <t>R80 Olav5 før CityNord</t>
         </is>
       </c>
       <c r="C145">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D145">
         <v>6</v>
       </c>
       <c r="E145">
-        <v>99.74372664175119</v>
+        <v>99.90547645773026</v>
       </c>
       <c r="F145">
-        <v>99.74372664175119</v>
+        <v>99.90547645773026</v>
       </c>
       <c r="G145">
-        <v>8388</v>
+        <v>15507</v>
+      </c>
+      <c r="H145">
+        <v>9.66</v>
       </c>
     </row>
     <row r="146">
@@ -5862,16 +5886,16 @@
         <v>2024</v>
       </c>
       <c r="D146">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E146">
-        <v>99.95326556840752</v>
+        <v>99.65114718905139</v>
       </c>
       <c r="F146">
-        <v>99.95326556840752</v>
+        <v>99.65114718905139</v>
       </c>
       <c r="G146">
-        <v>7663</v>
+        <v>6722</v>
       </c>
     </row>
     <row r="147">
@@ -5889,16 +5913,16 @@
         <v>2024</v>
       </c>
       <c r="D147">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E147">
-        <v>99.78756708407872</v>
+        <v>99.79185638090283</v>
       </c>
       <c r="F147">
-        <v>99.78756708407872</v>
+        <v>99.79185638090283</v>
       </c>
       <c r="G147">
-        <v>8035</v>
+        <v>6959</v>
       </c>
     </row>
     <row r="148">
@@ -5916,16 +5940,16 @@
         <v>2024</v>
       </c>
       <c r="D148">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E148">
-        <v>99.76942587041735</v>
+        <v>77.28192070242831</v>
       </c>
       <c r="F148">
-        <v>99.76942587041734</v>
+        <v>99.82164906022774</v>
       </c>
       <c r="G148">
-        <v>7852</v>
+        <v>6696</v>
       </c>
     </row>
     <row r="149">
@@ -5943,16 +5967,16 @@
         <v>2024</v>
       </c>
       <c r="D149">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E149">
-        <v>99.7340425531915</v>
+        <v>99.76520309931909</v>
       </c>
       <c r="F149">
-        <v>99.7340425531915</v>
+        <v>99.76520309931909</v>
       </c>
       <c r="G149">
-        <v>8238</v>
+        <v>7773</v>
       </c>
     </row>
     <row r="150">
@@ -5970,16 +5994,16 @@
         <v>2024</v>
       </c>
       <c r="D150">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E150">
-        <v>99.77467327625055</v>
+        <v>99.72764412165229</v>
       </c>
       <c r="F150">
-        <v>99.77467327625055</v>
+        <v>99.72764412165229</v>
       </c>
       <c r="G150">
-        <v>8138</v>
+        <v>8008</v>
       </c>
     </row>
     <row r="151">
@@ -5997,16 +6021,16 @@
         <v>2024</v>
       </c>
       <c r="D151">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E151">
-        <v>99.75683890577507</v>
+        <v>99.74372664175119</v>
       </c>
       <c r="F151">
-        <v>99.75683890577508</v>
+        <v>99.74372664175119</v>
       </c>
       <c r="G151">
-        <v>7630</v>
+        <v>8388</v>
       </c>
     </row>
     <row r="152">
@@ -6021,22 +6045,19 @@
         </is>
       </c>
       <c r="C152">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D152">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E152">
-        <v>99.73166368515206</v>
+        <v>99.95326556840752</v>
       </c>
       <c r="F152">
-        <v>99.73166368515206</v>
+        <v>99.95326556840752</v>
       </c>
       <c r="G152">
-        <v>6964</v>
-      </c>
-      <c r="H152">
-        <v>3.03</v>
+        <v>7663</v>
       </c>
     </row>
     <row r="153">
@@ -6051,22 +6072,19 @@
         </is>
       </c>
       <c r="C153">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D153">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E153">
-        <v>99.81041456016177</v>
+        <v>99.78756708407872</v>
       </c>
       <c r="F153">
-        <v>99.81041456016177</v>
+        <v>99.78756708407872</v>
       </c>
       <c r="G153">
-        <v>7107</v>
-      </c>
-      <c r="H153">
-        <v>2.22</v>
+        <v>8035</v>
       </c>
     </row>
     <row r="154">
@@ -6081,22 +6099,19 @@
         </is>
       </c>
       <c r="C154">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D154">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E154">
-        <v>99.86746189529489</v>
+        <v>99.76942587041735</v>
       </c>
       <c r="F154">
-        <v>99.86746189529489</v>
+        <v>99.76942587041734</v>
       </c>
       <c r="G154">
-        <v>6761</v>
-      </c>
-      <c r="H154">
-        <v>1.33</v>
+        <v>7852</v>
       </c>
     </row>
     <row r="155">
@@ -6111,22 +6126,19 @@
         </is>
       </c>
       <c r="C155">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D155">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E155">
-        <v>99.88745075970738</v>
+        <v>99.7340425531915</v>
       </c>
       <c r="F155">
-        <v>99.88745075970738</v>
+        <v>99.7340425531915</v>
       </c>
       <c r="G155">
-        <v>6377</v>
-      </c>
-      <c r="H155">
-        <v>-18.15</v>
+        <v>8238</v>
       </c>
     </row>
     <row r="156">
@@ -6141,211 +6153,226 @@
         </is>
       </c>
       <c r="C156">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D156">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E156">
-        <v>96.61224010337132</v>
+        <v>99.77467327625055</v>
       </c>
       <c r="F156">
-        <v>99.84729237636556</v>
+        <v>99.77467327625055</v>
       </c>
       <c r="G156">
-        <v>7576</v>
-      </c>
-      <c r="H156">
-        <v>-4.82</v>
+        <v>8138</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>19592V885287</t>
+          <t>77027V1207593</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Thallerkrysset</t>
+          <t>Sjøgata</t>
         </is>
       </c>
       <c r="C157">
         <v>2024</v>
       </c>
       <c r="D157">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E157">
-        <v>99.97885388031297</v>
+        <v>99.75683890577507</v>
       </c>
       <c r="F157">
-        <v>99.97885388031297</v>
+        <v>99.75683890577508</v>
       </c>
       <c r="G157">
-        <v>8812</v>
+        <v>7630</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>19592V885287</t>
+          <t>77027V1207593</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Thallerkrysset</t>
+          <t>Sjøgata</t>
         </is>
       </c>
       <c r="C158">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D158">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E158">
-        <v>99.98973832734735</v>
+        <v>99.73166368515206</v>
       </c>
       <c r="F158">
-        <v>99.98973832734735</v>
+        <v>99.73166368515206</v>
       </c>
       <c r="G158">
-        <v>9050</v>
+        <v>6964</v>
+      </c>
+      <c r="H158">
+        <v>3.03</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>19592V885287</t>
+          <t>77027V1207593</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Thallerkrysset</t>
+          <t>Sjøgata</t>
         </is>
       </c>
       <c r="C159">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D159">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E159">
-        <v>99.9563271099465</v>
+        <v>99.81041456016177</v>
       </c>
       <c r="F159">
-        <v>99.9563271099465</v>
+        <v>99.81041456016177</v>
       </c>
       <c r="G159">
-        <v>8542</v>
+        <v>7107</v>
+      </c>
+      <c r="H159">
+        <v>2.22</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>19592V885287</t>
+          <t>77027V1207593</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Thallerkrysset</t>
+          <t>Sjøgata</t>
         </is>
       </c>
       <c r="C160">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D160">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E160">
-        <v>99.97136311569301</v>
+        <v>99.86746189529489</v>
       </c>
       <c r="F160">
-        <v>99.97136311569301</v>
+        <v>99.86746189529489</v>
       </c>
       <c r="G160">
-        <v>9746</v>
+        <v>6761</v>
+      </c>
+      <c r="H160">
+        <v>1.33</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>19592V885287</t>
+          <t>77027V1207593</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Thallerkrysset</t>
+          <t>Sjøgata</t>
         </is>
       </c>
       <c r="C161">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D161">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E161">
-        <v>96.75184427767356</v>
+        <v>99.88745075970738</v>
       </c>
       <c r="F161">
-        <v>99.98123827392121</v>
+        <v>99.88745075970738</v>
       </c>
       <c r="G161">
-        <v>9843</v>
+        <v>6377</v>
+      </c>
+      <c r="H161">
+        <v>-18.15</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>19592V885287</t>
+          <t>77027V1207593</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Thallerkrysset</t>
+          <t>Sjøgata</t>
         </is>
       </c>
       <c r="C162">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D162">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E162">
-        <v>99.99098530604886</v>
+        <v>96.61224010337132</v>
       </c>
       <c r="F162">
-        <v>99.99098530604886</v>
+        <v>99.84729237636556</v>
       </c>
       <c r="G162">
-        <v>10073</v>
+        <v>7576</v>
+      </c>
+      <c r="H162">
+        <v>-4.82</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>19592V885287</t>
+          <t>77027V1207593</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Thallerkrysset</t>
+          <t>Sjøgata</t>
         </is>
       </c>
       <c r="C163">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D163">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E163">
-        <v>99.98983326555509</v>
+        <v>99.92112676056338</v>
       </c>
       <c r="F163">
-        <v>99.98983326555511</v>
+        <v>99.92112676056338</v>
       </c>
       <c r="G163">
-        <v>8893</v>
+        <v>7759</v>
+      </c>
+      <c r="H163">
+        <v>-7.85</v>
       </c>
     </row>
     <row r="164">
@@ -6363,16 +6390,16 @@
         <v>2024</v>
       </c>
       <c r="D164">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E164">
-        <v>99.98067518418353</v>
+        <v>99.97885388031297</v>
       </c>
       <c r="F164">
-        <v>99.9906742516087</v>
+        <v>99.97885388031297</v>
       </c>
       <c r="G164">
-        <v>9775</v>
+        <v>8812</v>
       </c>
     </row>
     <row r="165">
@@ -6390,16 +6417,16 @@
         <v>2024</v>
       </c>
       <c r="D165">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E165">
-        <v>99.99031476997578</v>
+        <v>99.98973832734735</v>
       </c>
       <c r="F165">
-        <v>99.99031476997578</v>
+        <v>99.98973832734735</v>
       </c>
       <c r="G165">
-        <v>9444</v>
+        <v>9050</v>
       </c>
     </row>
     <row r="166">
@@ -6417,16 +6444,16 @@
         <v>2024</v>
       </c>
       <c r="D166">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E166">
-        <v>99.99002792181891</v>
+        <v>99.9563271099465</v>
       </c>
       <c r="F166">
-        <v>99.99002792181891</v>
+        <v>99.9563271099465</v>
       </c>
       <c r="G166">
-        <v>9221</v>
+        <v>8542</v>
       </c>
     </row>
     <row r="167">
@@ -6444,16 +6471,16 @@
         <v>2024</v>
       </c>
       <c r="D167">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E167">
-        <v>99.990140011832</v>
+        <v>99.97136311569301</v>
       </c>
       <c r="F167">
-        <v>99.99014001183198</v>
+        <v>99.97136311569301</v>
       </c>
       <c r="G167">
-        <v>9401</v>
+        <v>9746</v>
       </c>
     </row>
     <row r="168">
@@ -6471,16 +6498,16 @@
         <v>2024</v>
       </c>
       <c r="D168">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E168">
-        <v>99.97837370242215</v>
+        <v>96.75184427767356</v>
       </c>
       <c r="F168">
-        <v>99.97837370242215</v>
+        <v>99.98123827392121</v>
       </c>
       <c r="G168">
-        <v>8704</v>
+        <v>9843</v>
       </c>
     </row>
     <row r="169">
@@ -6495,22 +6522,19 @@
         </is>
       </c>
       <c r="C169">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D169">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E169">
-        <v>99.98951232302045</v>
+        <v>99.99098530604886</v>
       </c>
       <c r="F169">
-        <v>99.98951232302045</v>
+        <v>99.99098530604886</v>
       </c>
       <c r="G169">
-        <v>8812</v>
-      </c>
-      <c r="H169">
-        <v>-0.12</v>
+        <v>10073</v>
       </c>
     </row>
     <row r="170">
@@ -6525,22 +6549,19 @@
         </is>
       </c>
       <c r="C170">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D170">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E170">
-        <v>99.98985698346686</v>
+        <v>99.98983326555509</v>
       </c>
       <c r="F170">
-        <v>99.98985698346688</v>
+        <v>99.98983326555511</v>
       </c>
       <c r="G170">
-        <v>9168</v>
-      </c>
-      <c r="H170">
-        <v>1.51</v>
+        <v>8893</v>
       </c>
     </row>
     <row r="171">
@@ -6555,22 +6576,19 @@
         </is>
       </c>
       <c r="C171">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D171">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E171">
-        <v>99.98962655601662</v>
+        <v>99.98067518418353</v>
       </c>
       <c r="F171">
-        <v>99.9896265560166</v>
+        <v>99.9906742516087</v>
       </c>
       <c r="G171">
-        <v>8959</v>
-      </c>
-      <c r="H171">
-        <v>4.91</v>
+        <v>9775</v>
       </c>
     </row>
     <row r="172">
@@ -6585,22 +6603,19 @@
         </is>
       </c>
       <c r="C172">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D172">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E172">
-        <v>99.9678869621066</v>
+        <v>99.99031476997578</v>
       </c>
       <c r="F172">
-        <v>99.9678869621066</v>
+        <v>99.99031476997578</v>
       </c>
       <c r="G172">
-        <v>8684</v>
-      </c>
-      <c r="H172">
-        <v>-10.89</v>
+        <v>9444</v>
       </c>
     </row>
     <row r="173">
@@ -6615,22 +6630,253 @@
         </is>
       </c>
       <c r="C173">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D173">
+        <v>10</v>
+      </c>
+      <c r="E173">
+        <v>99.99002792181891</v>
+      </c>
+      <c r="F173">
+        <v>99.99002792181891</v>
+      </c>
+      <c r="G173">
+        <v>9221</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>19592V885287</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Thallerkrysset</t>
+        </is>
+      </c>
+      <c r="C174">
+        <v>2024</v>
+      </c>
+      <c r="D174">
+        <v>11</v>
+      </c>
+      <c r="E174">
+        <v>99.990140011832</v>
+      </c>
+      <c r="F174">
+        <v>99.99014001183198</v>
+      </c>
+      <c r="G174">
+        <v>9401</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>19592V885287</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Thallerkrysset</t>
+        </is>
+      </c>
+      <c r="C175">
+        <v>2024</v>
+      </c>
+      <c r="D175">
+        <v>12</v>
+      </c>
+      <c r="E175">
+        <v>99.97837370242215</v>
+      </c>
+      <c r="F175">
+        <v>99.97837370242215</v>
+      </c>
+      <c r="G175">
+        <v>8704</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>19592V885287</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Thallerkrysset</t>
+        </is>
+      </c>
+      <c r="C176">
+        <v>2025</v>
+      </c>
+      <c r="D176">
+        <v>1</v>
+      </c>
+      <c r="E176">
+        <v>99.98951232302045</v>
+      </c>
+      <c r="F176">
+        <v>99.98951232302045</v>
+      </c>
+      <c r="G176">
+        <v>8812</v>
+      </c>
+      <c r="H176">
+        <v>-0.12</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>19592V885287</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Thallerkrysset</t>
+        </is>
+      </c>
+      <c r="C177">
+        <v>2025</v>
+      </c>
+      <c r="D177">
+        <v>2</v>
+      </c>
+      <c r="E177">
+        <v>99.98985698346686</v>
+      </c>
+      <c r="F177">
+        <v>99.98985698346688</v>
+      </c>
+      <c r="G177">
+        <v>9168</v>
+      </c>
+      <c r="H177">
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>19592V885287</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Thallerkrysset</t>
+        </is>
+      </c>
+      <c r="C178">
+        <v>2025</v>
+      </c>
+      <c r="D178">
+        <v>3</v>
+      </c>
+      <c r="E178">
+        <v>99.98962655601662</v>
+      </c>
+      <c r="F178">
+        <v>99.9896265560166</v>
+      </c>
+      <c r="G178">
+        <v>8959</v>
+      </c>
+      <c r="H178">
+        <v>4.91</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>19592V885287</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Thallerkrysset</t>
+        </is>
+      </c>
+      <c r="C179">
+        <v>2025</v>
+      </c>
+      <c r="D179">
+        <v>4</v>
+      </c>
+      <c r="E179">
+        <v>99.9678869621066</v>
+      </c>
+      <c r="F179">
+        <v>99.9678869621066</v>
+      </c>
+      <c r="G179">
+        <v>8684</v>
+      </c>
+      <c r="H179">
+        <v>-10.89</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>19592V885287</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Thallerkrysset</t>
+        </is>
+      </c>
+      <c r="C180">
+        <v>2025</v>
+      </c>
+      <c r="D180">
         <v>5</v>
       </c>
-      <c r="E173">
+      <c r="E180">
         <v>99.97221450402888</v>
       </c>
-      <c r="F173">
+      <c r="F180">
         <v>99.9722145040289</v>
       </c>
-      <c r="G173">
+      <c r="G180">
         <v>9909</v>
       </c>
-      <c r="H173">
+      <c r="H180">
         <v>0.05</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>19592V885287</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Thallerkrysset</t>
+        </is>
+      </c>
+      <c r="C181">
+        <v>2025</v>
+      </c>
+      <c r="D181">
+        <v>6</v>
+      </c>
+      <c r="E181">
+        <v>99.9637615510056</v>
+      </c>
+      <c r="F181">
+        <v>99.96376155100562</v>
+      </c>
+      <c r="G181">
+        <v>9968</v>
+      </c>
+      <c r="H181">
+        <v>-1.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>